<commit_message>
somases + trancamento parcial
</commit_message>
<xml_diff>
--- a/2.Excel/hands-on/6.Funcoes_Mercado/4.SOMA.SES/1.Funcao_SOMA.SES.xlsx
+++ b/2.Excel/hands-on/6.Funcoes_Mercado/4.SOMA.SES/1.Funcao_SOMA.SES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projetos para Github\Hashtag\2.Excel\hands-on\6.Funcoes_Mercado\4.SOMA.SES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65407F75-F313-41A0-8F93-C5784E07F684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9336C63-C09D-42B2-95AA-84EC6481E8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12180" yWindow="120" windowWidth="10896" windowHeight="12792" xr2:uid="{3D2557DA-CD0B-48AD-8EFD-8912689B8782}"/>
+    <workbookView xWindow="12180" yWindow="120" windowWidth="10896" windowHeight="12792" activeTab="1" xr2:uid="{3D2557DA-CD0B-48AD-8EFD-8912689B8782}"/>
   </bookViews>
   <sheets>
     <sheet name="SOMASES" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="79">
   <si>
     <t>Contratação</t>
   </si>
@@ -266,6 +266,15 @@
   </si>
   <si>
     <t>amarela</t>
+  </si>
+  <si>
+    <t>Produto 31</t>
+  </si>
+  <si>
+    <t>Produto 32</t>
+  </si>
+  <si>
+    <t>Produto 33</t>
   </si>
 </sst>
 </file>
@@ -379,7 +388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -414,6 +423,9 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -731,7 +743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37263547-D7E7-4AC6-B262-BC90CCAE7898}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -1019,9 +1031,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29FEF772-DFD0-4036-8B65-DBF82BF00CE4}">
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1112,7 +1126,17 @@
       <c r="E4" s="5">
         <v>1856</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="16">
+        <f>SUMIFS(E:E,B:B,J4)</f>
+        <v>9236</v>
+      </c>
+      <c r="J4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4">
+        <f>SUMIF(B:B,J4,E:E)</f>
+        <v>9236</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1196,7 +1220,10 @@
       <c r="E8" s="5">
         <v>2391</v>
       </c>
-      <c r="H8" s="7"/>
+      <c r="H8" s="7">
+        <f>SUMIFS(E:E,B:B,"Alemanha",D:D,"Puma")</f>
+        <v>271</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1280,7 +1307,10 @@
         <v>1945</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="H12" s="7"/>
+      <c r="H12" s="16">
+        <f>SUMIFS(E:E,C:C,"&gt;=01/01/2028",C:C,"&lt;=31/12/2029")</f>
+        <v>10606</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1405,12 +1435,30 @@
       <c r="H17" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
+      <c r="I17" s="10">
+        <f>SUMIFS($E:$E,$B:$B,$H17,$D:$D,I$16)</f>
+        <v>7204</v>
+      </c>
+      <c r="J17" s="10">
+        <f t="shared" ref="J17:N21" si="0">SUMIFS($E:$E,$B:$B,$H17,$D:$D,J$16)</f>
+        <v>6052</v>
+      </c>
+      <c r="K17" s="10">
+        <f t="shared" si="0"/>
+        <v>6856</v>
+      </c>
+      <c r="L17" s="10">
+        <f t="shared" si="0"/>
+        <v>2568</v>
+      </c>
+      <c r="M17" s="10">
+        <f t="shared" si="0"/>
+        <v>271</v>
+      </c>
+      <c r="N17" s="10">
+        <f t="shared" si="0"/>
+        <v>949</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -1431,12 +1479,30 @@
       <c r="H18" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
+      <c r="I18" s="10">
+        <f t="shared" ref="I18:I21" si="1">SUMIFS($E:$E,$B:$B,$H18,$D:$D,I$16)</f>
+        <v>2391</v>
+      </c>
+      <c r="J18" s="10">
+        <f t="shared" si="0"/>
+        <v>2423</v>
+      </c>
+      <c r="K18" s="10">
+        <f t="shared" si="0"/>
+        <v>1285</v>
+      </c>
+      <c r="L18" s="10">
+        <f t="shared" si="0"/>
+        <v>802</v>
+      </c>
+      <c r="M18" s="10">
+        <f t="shared" si="0"/>
+        <v>1945</v>
+      </c>
+      <c r="N18" s="10">
+        <f t="shared" si="0"/>
+        <v>212</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -1457,12 +1523,30 @@
       <c r="H19" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
+      <c r="I19" s="10">
+        <f t="shared" si="1"/>
+        <v>1771</v>
+      </c>
+      <c r="J19" s="10">
+        <f t="shared" si="0"/>
+        <v>1423</v>
+      </c>
+      <c r="K19" s="10">
+        <f t="shared" si="0"/>
+        <v>1457</v>
+      </c>
+      <c r="L19" s="10">
+        <f t="shared" si="0"/>
+        <v>2528</v>
+      </c>
+      <c r="M19" s="10">
+        <f t="shared" si="0"/>
+        <v>603</v>
+      </c>
+      <c r="N19" s="10">
+        <f t="shared" si="0"/>
+        <v>1454</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -1483,12 +1567,30 @@
       <c r="H20" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
+      <c r="I20" s="10">
+        <f t="shared" si="1"/>
+        <v>1760</v>
+      </c>
+      <c r="J20" s="10">
+        <f t="shared" si="0"/>
+        <v>205</v>
+      </c>
+      <c r="K20" s="10">
+        <f t="shared" si="0"/>
+        <v>1703</v>
+      </c>
+      <c r="L20" s="10">
+        <f t="shared" si="0"/>
+        <v>2266</v>
+      </c>
+      <c r="M20" s="10">
+        <f t="shared" si="0"/>
+        <v>733</v>
+      </c>
+      <c r="N20" s="10">
+        <f t="shared" si="0"/>
+        <v>2181</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -1509,12 +1611,30 @@
       <c r="H21" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
+      <c r="I21" s="10">
+        <f t="shared" si="1"/>
+        <v>293</v>
+      </c>
+      <c r="J21" s="10">
+        <f t="shared" si="0"/>
+        <v>2397</v>
+      </c>
+      <c r="K21" s="10">
+        <f t="shared" si="0"/>
+        <v>2340</v>
+      </c>
+      <c r="L21" s="10">
+        <f t="shared" si="0"/>
+        <v>865</v>
+      </c>
+      <c r="M21" s="10">
+        <f t="shared" si="0"/>
+        <v>229</v>
+      </c>
+      <c r="N21" s="10">
+        <f t="shared" si="0"/>
+        <v>2811</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -1684,6 +1804,57 @@
       </c>
       <c r="E31" s="5">
         <v>2811</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="4">
+        <v>45557</v>
+      </c>
+      <c r="D32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="5">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="4">
+        <v>45557</v>
+      </c>
+      <c r="D33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" s="5">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="4">
+        <v>45557</v>
+      </c>
+      <c r="D34" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="5">
+        <v>5000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>